<commit_message>
Modification for git repo
</commit_message>
<xml_diff>
--- a/public/Audit.xlsx
+++ b/public/Audit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fernando\Documents\WD\email-node\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2C3C20-04E4-4BEF-9C0A-587A7137B447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DF2C3F-5D29-45BB-A6AF-F31BFC707BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="1305" windowWidth="16200" windowHeight="9270" xr2:uid="{6EDB370D-84F7-4B74-81C0-A51E4EDB49E3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6EDB370D-84F7-4B74-81C0-A51E4EDB49E3}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerList" sheetId="1" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>SolFecha</t>
   </si>
   <si>
-    <t>Oscar Castro</t>
-  </si>
-  <si>
     <t>Ketal Supermercados</t>
   </si>
   <si>
@@ -240,7 +237,10 @@
     <t>KETAL20220211selfdeclaration.pdf</t>
   </si>
   <si>
-    <t>ocastro@ketal.com.bo;rcondori@ketal.com.bo</t>
+    <t>Jose Luis Murillo</t>
+  </si>
+  <si>
+    <t>jmurillo@ketal.com.bo; rcondori@ketal.com.bo</t>
   </si>
 </sst>
 </file>
@@ -331,7 +331,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,7 +649,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,37 +1037,38 @@
         <v>1</v>
       </c>
       <c r="E8" s="6">
-        <v>44603</v>
+        <v>44607</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="J8" s="6">
         <v>44666</v>
       </c>
       <c r="L8" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="M8" t="s">
         <v>68</v>
       </c>
       <c r="N8" t="s">
+        <v>64</v>
+      </c>
+      <c r="O8" t="s">
         <v>65</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>66</v>
-      </c>
-      <c r="P8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E9" s="10"/>
       <c r="I9" s="11"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>